<commit_message>
atualizacao do documento de homologacao
</commit_message>
<xml_diff>
--- a/docs/(Estre - Geotecnia) Solicitações em Homologação.xlsx
+++ b/docs/(Estre - Geotecnia) Solicitações em Homologação.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michel.oliveira\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projetos\estre\EstreMonitoramento\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
   <si>
     <t>Aterro</t>
   </si>
@@ -189,10 +189,10 @@
     </r>
   </si>
   <si>
-    <t>Ok</t>
-  </si>
-  <si>
-    <t>Medir impacto no filtro / desktop: datetimepicker.html</t>
+    <t>Corrigido</t>
+  </si>
+  <si>
+    <t>Expliquei pro Vini o que precisa ser feito.</t>
   </si>
 </sst>
 </file>
@@ -248,7 +248,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -273,6 +273,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -362,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -419,6 +425,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -752,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,8 +930,8 @@
     </row>
     <row r="18" spans="2:6" ht="120" x14ac:dyDescent="0.25">
       <c r="B18" s="18"/>
-      <c r="C18" s="6" t="s">
-        <v>12</v>
+      <c r="C18" s="20" t="s">
+        <v>36</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>35</v>
@@ -930,23 +939,17 @@
       <c r="E18" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="19" spans="2:6" ht="90" x14ac:dyDescent="0.25">
       <c r="B19" s="18"/>
-      <c r="C19" s="6" t="s">
-        <v>12</v>
+      <c r="C19" s="20" t="s">
+        <v>36</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="30" x14ac:dyDescent="0.25">
@@ -966,8 +969,8 @@
     </row>
     <row r="21" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B21" s="18"/>
-      <c r="C21" s="6" t="s">
-        <v>12</v>
+      <c r="C21" s="20" t="s">
+        <v>36</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>33</v>
@@ -975,23 +978,17 @@
       <c r="E21" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="4" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="22" spans="2:6" ht="180" x14ac:dyDescent="0.25">
       <c r="B22" s="19"/>
-      <c r="C22" s="6" t="s">
-        <v>12</v>
+      <c r="C22" s="20" t="s">
+        <v>36</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -1013,6 +1010,9 @@
       <c r="E24" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="F24" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="25" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B25" s="19"/>
@@ -1024,6 +1024,9 @@
       </c>
       <c r="E25" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="2:6" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
ajustes planilha de homologação
</commit_message>
<xml_diff>
--- a/docs/(Estre - Geotecnia) Solicitações em Homologação.xlsx
+++ b/docs/(Estre - Geotecnia) Solicitações em Homologação.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
   <si>
     <t>Aterro</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>Expliquei pro Vini o que precisa ser feito.</t>
+  </si>
+  <si>
+    <t>Aguardando definição do cliente.</t>
   </si>
 </sst>
 </file>
@@ -248,7 +251,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -279,6 +282,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -368,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -428,6 +437,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -761,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,7 +782,7 @@
     <col min="1" max="1" width="9" style="4"/>
     <col min="2" max="2" width="26.28515625" style="5" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="52.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="66.7109375" style="4" customWidth="1"/>
     <col min="5" max="5" width="27.42578125" style="4" customWidth="1"/>
     <col min="6" max="6" width="35" style="4" customWidth="1"/>
     <col min="7" max="16384" width="9" style="4"/>
@@ -830,8 +842,8 @@
       <c r="B8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>12</v>
+      <c r="C8" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -850,8 +862,8 @@
       <c r="B10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>12</v>
+      <c r="C10" s="21" t="s">
+        <v>38</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>17</v>
@@ -954,8 +966,8 @@
     </row>
     <row r="20" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="19"/>
-      <c r="C20" s="6" t="s">
-        <v>12</v>
+      <c r="C20" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>25</v>
@@ -1001,8 +1013,8 @@
       <c r="B24" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>12</v>
+      <c r="C24" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>21</v>
@@ -1016,8 +1028,8 @@
     </row>
     <row r="25" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B25" s="20"/>
-      <c r="C25" s="6" t="s">
-        <v>12</v>
+      <c r="C25" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>22</v>
@@ -1117,7 +1129,7 @@
     <mergeCell ref="B17:B22"/>
     <mergeCell ref="B24:B25"/>
   </mergeCells>
-  <conditionalFormatting sqref="C6:C15 C17:C33">
+  <conditionalFormatting sqref="C17:C33 C6:C15">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Nok"</formula>
     </cfRule>

</xml_diff>